<commit_message>
Fourth Commit - Legendary Fire Pokemon Data CSV and workbook updated
</commit_message>
<xml_diff>
--- a/legendary_fire_pokemon.xlsx
+++ b/legendary_fire_pokemon.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,324 +434,305 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Type 1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Type 1</t>
+          <t>Type 2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Type 2</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Attack</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Attack</t>
+          <t>Defense</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Defense</t>
+          <t>Sp. Atk</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Sp. Atk</t>
+          <t>Sp. Def</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Sp. Def</t>
+          <t>Speed</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Speed</t>
+          <t>Generation</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Generation</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Legendary</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
         <v>146</v>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Moltres</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Moltres</t>
+          <t>Fire</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fire</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>Flying</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>700</v>
+      </c>
       <c r="F2" t="n">
-        <v>700</v>
+        <v>90</v>
       </c>
       <c r="G2" t="n">
+        <v>200</v>
+      </c>
+      <c r="H2" t="n">
+        <v>200</v>
+      </c>
+      <c r="I2" t="n">
+        <v>125</v>
+      </c>
+      <c r="J2" t="n">
+        <v>85</v>
+      </c>
+      <c r="K2" t="n">
         <v>90</v>
       </c>
-      <c r="H2" t="n">
-        <v>200</v>
-      </c>
-      <c r="I2" t="n">
-        <v>200</v>
-      </c>
-      <c r="J2" t="n">
-        <v>125</v>
-      </c>
-      <c r="K2" t="n">
-        <v>85</v>
-      </c>
       <c r="L2" t="n">
-        <v>90</v>
-      </c>
-      <c r="M2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" t="b">
+      <c r="M2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>263</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n">
         <v>244</v>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Entei</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Entei</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>Fire</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>665</v>
+      </c>
       <c r="F3" t="n">
-        <v>665</v>
+        <v>115</v>
       </c>
       <c r="G3" t="n">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="H3" t="n">
         <v>200</v>
       </c>
       <c r="I3" t="n">
-        <v>200</v>
+        <v>90</v>
       </c>
       <c r="J3" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="K3" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="L3" t="n">
-        <v>100</v>
-      </c>
-      <c r="M3" t="n">
         <v>2</v>
       </c>
-      <c r="N3" t="b">
+      <c r="M3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>270</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="n">
         <v>250</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ho-oh</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ho-oh</t>
+          <t>Fire</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fire</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t>Flying</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>754</v>
+      </c>
       <c r="F4" t="n">
-        <v>754</v>
+        <v>106</v>
       </c>
       <c r="G4" t="n">
-        <v>106</v>
+        <v>200</v>
       </c>
       <c r="H4" t="n">
         <v>200</v>
       </c>
       <c r="I4" t="n">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="J4" t="n">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="K4" t="n">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="L4" t="n">
-        <v>90</v>
-      </c>
-      <c r="M4" t="n">
         <v>2</v>
       </c>
-      <c r="N4" t="b">
+      <c r="M4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>542</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" t="n">
         <v>485</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Heatran</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Heatran</t>
+          <t>Fire</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fire</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
           <t>Steel</t>
         </is>
       </c>
+      <c r="E5" t="n">
+        <v>713</v>
+      </c>
       <c r="F5" t="n">
-        <v>713</v>
+        <v>91</v>
       </c>
       <c r="G5" t="n">
-        <v>91</v>
+        <v>200</v>
       </c>
       <c r="H5" t="n">
         <v>200</v>
       </c>
       <c r="I5" t="n">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="J5" t="n">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="K5" t="n">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="L5" t="n">
-        <v>77</v>
-      </c>
-      <c r="M5" t="n">
         <v>4</v>
       </c>
-      <c r="N5" t="b">
+      <c r="M5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>799</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" t="n">
         <v>721</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Volcanion</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Volcanion</t>
+          <t>Fire</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Fire</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
           <t>Water</t>
         </is>
       </c>
+      <c r="E6" t="n">
+        <v>690</v>
+      </c>
       <c r="F6" t="n">
-        <v>690</v>
+        <v>80</v>
       </c>
       <c r="G6" t="n">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="H6" t="n">
         <v>200</v>
       </c>
       <c r="I6" t="n">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="J6" t="n">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="K6" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="L6" t="n">
-        <v>70</v>
-      </c>
-      <c r="M6" t="n">
         <v>6</v>
       </c>
-      <c r="N6" t="b">
+      <c r="M6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -764,7 +745,6 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>